<commit_message>
check markov property for all majors, science and technolgy and selected majors data
</commit_message>
<xml_diff>
--- a/All Major/All Major_fall.xlsx
+++ b/All Major/All Major_fall.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>Major Beginning of Semester</t>
   </si>
@@ -163,10 +163,13 @@
     <t>MSSP-BS</t>
   </si>
   <si>
-    <t>Others</t>
+    <t>NURS-BSN</t>
   </si>
   <si>
     <t>SCMT-BS</t>
+  </si>
+  <si>
+    <t>SPAN-BA</t>
   </si>
   <si>
     <t>SO</t>
@@ -11006,7 +11009,7 @@
         <v>0</v>
       </c>
       <c r="E524" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F524" t="n">
         <v>2.091</v>
@@ -11736,7 +11739,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="n">
         <v>3.204</v>
@@ -11756,7 +11759,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="n">
         <v>2.977</v>
@@ -11776,7 +11779,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="n">
         <v>3.923</v>
@@ -11796,7 +11799,7 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" t="n">
         <v>2.938</v>
@@ -11816,7 +11819,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" t="n">
         <v>2.917</v>
@@ -11836,7 +11839,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" t="n">
         <v>3.406</v>
@@ -11856,7 +11859,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" t="n">
         <v>2.313</v>
@@ -11876,7 +11879,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" t="n">
         <v>2.545</v>
@@ -11896,7 +11899,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" t="n">
         <v>2.431</v>
@@ -11916,7 +11919,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" t="n">
         <v>2.392</v>
@@ -11936,7 +11939,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" t="n">
         <v>3</v>
@@ -11956,7 +11959,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" t="n">
         <v>3.067</v>
@@ -11976,7 +11979,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" t="n">
         <v>2.588</v>
@@ -11996,7 +11999,7 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" t="n">
         <v>2.286</v>
@@ -12016,7 +12019,7 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" t="n">
         <v>3.625</v>
@@ -12036,7 +12039,7 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" t="n">
         <v>2.319</v>
@@ -12056,7 +12059,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" t="n">
         <v>3.184</v>
@@ -12076,7 +12079,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" t="n">
         <v>2.278</v>
@@ -12096,7 +12099,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D20" t="n">
         <v>2.704</v>
@@ -12116,7 +12119,7 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D21" t="n">
         <v>2.903</v>
@@ -12136,7 +12139,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" t="n">
         <v>3.031</v>
@@ -12156,7 +12159,7 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D23" t="n">
         <v>1.365</v>
@@ -12176,7 +12179,7 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" t="n">
         <v>3.563</v>
@@ -12196,7 +12199,7 @@
         <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25" t="n">
         <v>2.273</v>
@@ -12216,7 +12219,7 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D26" t="n">
         <v>2.714</v>
@@ -12236,7 +12239,7 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D27" t="n">
         <v>2.025</v>
@@ -12256,7 +12259,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D28" t="n">
         <v>4</v>
@@ -12276,7 +12279,7 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29" t="n">
         <v>3</v>
@@ -12296,7 +12299,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D30" t="n">
         <v>3.909</v>
@@ -12316,7 +12319,7 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D31" t="n">
         <v>2.515</v>
@@ -12336,7 +12339,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D32" t="n">
         <v>3.119</v>
@@ -12356,7 +12359,7 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D33" t="n">
         <v>3.3</v>
@@ -12376,7 +12379,7 @@
         <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D34" t="n">
         <v>3.773</v>
@@ -12396,7 +12399,7 @@
         <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D35" t="n">
         <v>1.898</v>
@@ -12416,7 +12419,7 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D36" t="n">
         <v>2.032</v>
@@ -12436,7 +12439,7 @@
         <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D37" t="n">
         <v>3.921</v>
@@ -12456,7 +12459,7 @@
         <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D38" t="n">
         <v>2.342</v>
@@ -12476,7 +12479,7 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D39" t="n">
         <v>2.6</v>
@@ -12496,7 +12499,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D40" t="n">
         <v>2.929</v>
@@ -12516,7 +12519,7 @@
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D41" t="n">
         <v>3.1</v>
@@ -12536,7 +12539,7 @@
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D42" t="n">
         <v>2.784</v>
@@ -12556,7 +12559,7 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D43" t="n">
         <v>4</v>
@@ -12576,7 +12579,7 @@
         <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D44" t="n">
         <v>2.855</v>
@@ -12596,7 +12599,7 @@
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D45" t="n">
         <v>2.967</v>
@@ -12616,7 +12619,7 @@
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D46" t="n">
         <v>3.755</v>
@@ -12636,7 +12639,7 @@
         <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D47" t="n">
         <v>2</v>
@@ -12656,7 +12659,7 @@
         <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D48" t="n">
         <v>3.132</v>
@@ -12676,7 +12679,7 @@
         <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D49" t="n">
         <v>2.292</v>
@@ -12696,7 +12699,7 @@
         <v>36</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D50" t="n">
         <v>4</v>
@@ -12716,7 +12719,7 @@
         <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D51" t="n">
         <v>3.314</v>
@@ -12736,7 +12739,7 @@
         <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D52" t="n">
         <v>2.021</v>
@@ -12756,7 +12759,7 @@
         <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D53" t="n">
         <v>2.444</v>
@@ -12776,7 +12779,7 @@
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D54" t="n">
         <v>2.83</v>
@@ -12796,7 +12799,7 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D55" t="n">
         <v>1.333</v>
@@ -12816,7 +12819,7 @@
         <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D56" t="n">
         <v>3.444</v>
@@ -12836,7 +12839,7 @@
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D57" t="n">
         <v>2.643</v>
@@ -12856,7 +12859,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D58" t="n">
         <v>2.839</v>
@@ -12876,7 +12879,7 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D59" t="n">
         <v>2.342</v>
@@ -12896,7 +12899,7 @@
         <v>32</v>
       </c>
       <c r="C60" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D60" t="n">
         <v>2.909</v>
@@ -12916,7 +12919,7 @@
         <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D61" t="n">
         <v>2.481</v>
@@ -12936,7 +12939,7 @@
         <v>32</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D62" t="n">
         <v>3.067</v>
@@ -12956,7 +12959,7 @@
         <v>34</v>
       </c>
       <c r="C63" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D63" t="n">
         <v>2.846</v>
@@ -12976,7 +12979,7 @@
         <v>34</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D64" t="n">
         <v>3.071</v>
@@ -12996,7 +12999,7 @@
         <v>34</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D65" t="n">
         <v>3.488</v>
@@ -13016,7 +13019,7 @@
         <v>18</v>
       </c>
       <c r="C66" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D66" t="n">
         <v>2.455</v>
@@ -13036,7 +13039,7 @@
         <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D67" t="n">
         <v>3</v>
@@ -13056,7 +13059,7 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D68" t="n">
         <v>2.548</v>
@@ -13076,7 +13079,7 @@
         <v>38</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D69" t="n">
         <v>1.955</v>
@@ -13096,7 +13099,7 @@
         <v>38</v>
       </c>
       <c r="C70" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D70" t="n">
         <v>3.509</v>
@@ -13116,7 +13119,7 @@
         <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D71" t="n">
         <v>3.595</v>
@@ -13136,7 +13139,7 @@
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D72" t="n">
         <v>2.372</v>
@@ -13156,7 +13159,7 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D73" t="n">
         <v>2.136</v>
@@ -13176,7 +13179,7 @@
         <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D74" t="n">
         <v>2.574</v>
@@ -13196,7 +13199,7 @@
         <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D75" t="n">
         <v>2.18</v>
@@ -13216,7 +13219,7 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D76" t="n">
         <v>2.257</v>
@@ -13236,7 +13239,7 @@
         <v>39</v>
       </c>
       <c r="C77" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D77" t="n">
         <v>2.658</v>
@@ -13256,7 +13259,7 @@
         <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D78" t="n">
         <v>3.2</v>
@@ -13276,7 +13279,7 @@
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D79" t="n">
         <v>3.049</v>
@@ -13296,7 +13299,7 @@
         <v>42</v>
       </c>
       <c r="C80" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D80" t="n">
         <v>2.175</v>
@@ -13316,7 +13319,7 @@
         <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D81" t="n">
         <v>3.634</v>
@@ -13336,7 +13339,7 @@
         <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D82" t="n">
         <v>3.389</v>
@@ -13356,7 +13359,7 @@
         <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D83" t="n">
         <v>3.515</v>
@@ -13376,7 +13379,7 @@
         <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D84" t="n">
         <v>2.68</v>
@@ -13396,7 +13399,7 @@
         <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D85" t="n">
         <v>3.886</v>
@@ -13416,7 +13419,7 @@
         <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D86" t="n">
         <v>1.432</v>
@@ -13436,7 +13439,7 @@
         <v>45</v>
       </c>
       <c r="C87" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D87" t="n">
         <v>2.621</v>
@@ -13456,7 +13459,7 @@
         <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D88" t="n">
         <v>2.2</v>
@@ -13476,7 +13479,7 @@
         <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D89" t="n">
         <v>3.353</v>
@@ -13496,7 +13499,7 @@
         <v>20</v>
       </c>
       <c r="C90" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D90" t="n">
         <v>2.946</v>
@@ -13516,7 +13519,7 @@
         <v>21</v>
       </c>
       <c r="C91" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D91" t="n">
         <v>2.483</v>
@@ -13536,7 +13539,7 @@
         <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D92" t="n">
         <v>2.06</v>
@@ -13556,7 +13559,7 @@
         <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D93" t="n">
         <v>2.455</v>
@@ -13576,7 +13579,7 @@
         <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D94" t="n">
         <v>3</v>
@@ -13596,7 +13599,7 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D95" t="n">
         <v>2.561</v>
@@ -13616,7 +13619,7 @@
         <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D96" t="n">
         <v>2.036</v>
@@ -13636,7 +13639,7 @@
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D97" t="n">
         <v>3.105</v>
@@ -13656,7 +13659,7 @@
         <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D98" t="n">
         <v>2.218</v>
@@ -13676,7 +13679,7 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D99" t="n">
         <v>2.833</v>
@@ -13696,7 +13699,7 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D100" t="n">
         <v>2.862</v>
@@ -13716,7 +13719,7 @@
         <v>11</v>
       </c>
       <c r="C101" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D101" t="n">
         <v>2.625</v>
@@ -13736,7 +13739,7 @@
         <v>39</v>
       </c>
       <c r="C102" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D102" t="n">
         <v>2.86</v>
@@ -13756,7 +13759,7 @@
         <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D103" t="n">
         <v>2.359</v>
@@ -13776,7 +13779,7 @@
         <v>45</v>
       </c>
       <c r="C104" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D104" t="n">
         <v>3.152</v>
@@ -13796,7 +13799,7 @@
         <v>15</v>
       </c>
       <c r="C105" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D105" t="n">
         <v>1.63</v>
@@ -13816,7 +13819,7 @@
         <v>16</v>
       </c>
       <c r="C106" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D106" t="n">
         <v>2.5</v>
@@ -13836,7 +13839,7 @@
         <v>18</v>
       </c>
       <c r="C107" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D107" t="n">
         <v>2.211</v>
@@ -13856,7 +13859,7 @@
         <v>26</v>
       </c>
       <c r="C108" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D108" t="n">
         <v>1.944</v>
@@ -13876,7 +13879,7 @@
         <v>41</v>
       </c>
       <c r="C109" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D109" t="n">
         <v>2.566</v>
@@ -13896,7 +13899,7 @@
         <v>21</v>
       </c>
       <c r="C110" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D110" t="n">
         <v>3.426</v>
@@ -13916,13 +13919,13 @@
         <v>24</v>
       </c>
       <c r="C111" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D111" t="n">
         <v>2.388</v>
       </c>
       <c r="E111" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F111" t="n">
         <v>2.484</v>
@@ -13936,13 +13939,13 @@
         <v>24</v>
       </c>
       <c r="C112" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D112" t="n">
         <v>2.058</v>
       </c>
       <c r="E112" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F112" t="n">
         <v>2.141</v>
@@ -13956,7 +13959,7 @@
         <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D113" t="n">
         <v>3.273</v>
@@ -13976,7 +13979,7 @@
         <v>19</v>
       </c>
       <c r="C114" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D114" t="n">
         <v>3.519</v>
@@ -13996,7 +13999,7 @@
         <v>33</v>
       </c>
       <c r="C115" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D115" t="n">
         <v>2.058</v>
@@ -14016,7 +14019,7 @@
         <v>33</v>
       </c>
       <c r="C116" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D116" t="n">
         <v>1.952</v>
@@ -14036,7 +14039,7 @@
         <v>33</v>
       </c>
       <c r="C117" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D117" t="n">
         <v>2.759</v>
@@ -14056,7 +14059,7 @@
         <v>33</v>
       </c>
       <c r="C118" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D118" t="n">
         <v>2.767</v>
@@ -14076,7 +14079,7 @@
         <v>33</v>
       </c>
       <c r="C119" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D119" t="n">
         <v>2.425</v>
@@ -14096,7 +14099,7 @@
         <v>33</v>
       </c>
       <c r="C120" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D120" t="n">
         <v>3.781</v>
@@ -14116,7 +14119,7 @@
         <v>23</v>
       </c>
       <c r="C121" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D121" t="n">
         <v>2.903</v>
@@ -14136,7 +14139,7 @@
         <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D122" t="n">
         <v>2.357</v>
@@ -14156,7 +14159,7 @@
         <v>18</v>
       </c>
       <c r="C123" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D123" t="n">
         <v>2.788</v>
@@ -14176,7 +14179,7 @@
         <v>18</v>
       </c>
       <c r="C124" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D124" t="n">
         <v>3.517</v>
@@ -14196,7 +14199,7 @@
         <v>42</v>
       </c>
       <c r="C125" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D125" t="n">
         <v>2.432</v>
@@ -14216,7 +14219,7 @@
         <v>21</v>
       </c>
       <c r="C126" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D126" t="n">
         <v>3.375</v>
@@ -14236,7 +14239,7 @@
         <v>21</v>
       </c>
       <c r="C127" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D127" t="n">
         <v>3.921</v>
@@ -14256,7 +14259,7 @@
         <v>8</v>
       </c>
       <c r="C128" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D128" t="n">
         <v>2.149</v>
@@ -14276,7 +14279,7 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D129" t="n">
         <v>2.115</v>
@@ -14296,7 +14299,7 @@
         <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D130" t="n">
         <v>2.429</v>
@@ -14316,7 +14319,7 @@
         <v>22</v>
       </c>
       <c r="C131" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D131" t="n">
         <v>2.966</v>
@@ -14336,7 +14339,7 @@
         <v>14</v>
       </c>
       <c r="C132" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D132" t="n">
         <v>2.6</v>
@@ -14356,7 +14359,7 @@
         <v>30</v>
       </c>
       <c r="C133" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D133" t="n">
         <v>2.447</v>
@@ -14376,7 +14379,7 @@
         <v>30</v>
       </c>
       <c r="C134" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D134" t="n">
         <v>3.367</v>
@@ -14396,7 +14399,7 @@
         <v>26</v>
       </c>
       <c r="C135" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D135" t="n">
         <v>2.818</v>
@@ -14416,7 +14419,7 @@
         <v>12</v>
       </c>
       <c r="C136" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D136" t="n">
         <v>3.14</v>
@@ -14436,7 +14439,7 @@
         <v>12</v>
       </c>
       <c r="C137" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D137" t="n">
         <v>3.071</v>
@@ -14456,7 +14459,7 @@
         <v>12</v>
       </c>
       <c r="C138" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D138" t="n">
         <v>2.455</v>
@@ -14476,7 +14479,7 @@
         <v>12</v>
       </c>
       <c r="C139" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D139" t="n">
         <v>2.719</v>
@@ -14496,7 +14499,7 @@
         <v>21</v>
       </c>
       <c r="C140" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D140" t="n">
         <v>2.733</v>
@@ -14516,7 +14519,7 @@
         <v>24</v>
       </c>
       <c r="C141" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D141" t="n">
         <v>3.03</v>
@@ -14536,7 +14539,7 @@
         <v>24</v>
       </c>
       <c r="C142" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D142" t="n">
         <v>3.125</v>
@@ -14556,7 +14559,7 @@
         <v>9</v>
       </c>
       <c r="C143" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D143" t="n">
         <v>3.5</v>
@@ -14576,7 +14579,7 @@
         <v>9</v>
       </c>
       <c r="C144" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D144" t="n">
         <v>3.033</v>
@@ -14593,10 +14596,10 @@
         <v>616</v>
       </c>
       <c r="B145" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C145" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D145" t="n">
         <v>1.536</v>
@@ -14616,7 +14619,7 @@
         <v>30</v>
       </c>
       <c r="C146" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D146" t="n">
         <v>2.121</v>
@@ -14636,7 +14639,7 @@
         <v>16</v>
       </c>
       <c r="C147" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D147" t="n">
         <v>3.9</v>
@@ -14656,7 +14659,7 @@
         <v>17</v>
       </c>
       <c r="C148" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D148" t="n">
         <v>1.882</v>
@@ -14676,7 +14679,7 @@
         <v>18</v>
       </c>
       <c r="C149" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D149" t="n">
         <v>2.038</v>
@@ -14696,7 +14699,7 @@
         <v>18</v>
       </c>
       <c r="C150" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D150" t="n">
         <v>3.245</v>
@@ -14716,7 +14719,7 @@
         <v>18</v>
       </c>
       <c r="C151" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D151" t="n">
         <v>2.855</v>
@@ -14736,7 +14739,7 @@
         <v>18</v>
       </c>
       <c r="C152" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D152" t="n">
         <v>3.018</v>
@@ -14756,7 +14759,7 @@
         <v>21</v>
       </c>
       <c r="C153" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D153" t="n">
         <v>3.25</v>
@@ -14776,7 +14779,7 @@
         <v>7</v>
       </c>
       <c r="C154" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D154" t="n">
         <v>3.721</v>
@@ -14796,7 +14799,7 @@
         <v>13</v>
       </c>
       <c r="C155" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D155" t="n">
         <v>3</v>
@@ -14816,7 +14819,7 @@
         <v>7</v>
       </c>
       <c r="C156" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D156" t="n">
         <v>2.78</v>
@@ -14836,7 +14839,7 @@
         <v>8</v>
       </c>
       <c r="C157" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D157" t="n">
         <v>2.2</v>
@@ -14856,7 +14859,7 @@
         <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D158" t="n">
         <v>2</v>
@@ -14876,7 +14879,7 @@
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D159" t="n">
         <v>3.688</v>
@@ -14896,7 +14899,7 @@
         <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D160" t="n">
         <v>2.5</v>
@@ -14916,7 +14919,7 @@
         <v>12</v>
       </c>
       <c r="C161" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D161" t="n">
         <v>2.025</v>
@@ -14936,7 +14939,7 @@
         <v>39</v>
       </c>
       <c r="C162" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D162" t="n">
         <v>2.263</v>
@@ -14956,7 +14959,7 @@
         <v>22</v>
       </c>
       <c r="C163" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D163" t="n">
         <v>2.262</v>
@@ -14976,7 +14979,7 @@
         <v>22</v>
       </c>
       <c r="C164" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D164" t="n">
         <v>2.273</v>
@@ -14996,7 +14999,7 @@
         <v>22</v>
       </c>
       <c r="C165" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D165" t="n">
         <v>2.925</v>
@@ -15016,7 +15019,7 @@
         <v>22</v>
       </c>
       <c r="C166" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D166" t="n">
         <v>3.365</v>
@@ -15036,7 +15039,7 @@
         <v>29</v>
       </c>
       <c r="C167" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D167" t="n">
         <v>2.263</v>
@@ -15056,7 +15059,7 @@
         <v>14</v>
       </c>
       <c r="C168" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D168" t="n">
         <v>2.19</v>
@@ -15076,7 +15079,7 @@
         <v>25</v>
       </c>
       <c r="C169" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D169" t="n">
         <v>2.35</v>
@@ -15096,7 +15099,7 @@
         <v>17</v>
       </c>
       <c r="C170" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D170" t="n">
         <v>2.471</v>
@@ -15116,7 +15119,7 @@
         <v>17</v>
       </c>
       <c r="C171" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D171" t="n">
         <v>2.407</v>
@@ -15136,7 +15139,7 @@
         <v>18</v>
       </c>
       <c r="C172" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D172" t="n">
         <v>2.767</v>
@@ -15156,7 +15159,7 @@
         <v>33</v>
       </c>
       <c r="C173" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D173" t="n">
         <v>3.719</v>
@@ -15176,7 +15179,7 @@
         <v>21</v>
       </c>
       <c r="C174" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D174" t="n">
         <v>2.8</v>
@@ -15196,7 +15199,7 @@
         <v>7</v>
       </c>
       <c r="C175" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D175" t="n">
         <v>3.364</v>
@@ -15216,7 +15219,7 @@
         <v>7</v>
       </c>
       <c r="C176" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D176" t="n">
         <v>3.8</v>
@@ -15236,7 +15239,7 @@
         <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D177" t="n">
         <v>2.559</v>
@@ -15256,7 +15259,7 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D178" t="n">
         <v>3.464</v>
@@ -15276,7 +15279,7 @@
         <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D179" t="n">
         <v>2.909</v>
@@ -15296,7 +15299,7 @@
         <v>13</v>
       </c>
       <c r="C180" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D180" t="n">
         <v>3.615</v>
@@ -15316,7 +15319,7 @@
         <v>16</v>
       </c>
       <c r="C181" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D181" t="n">
         <v>2.945</v>
@@ -15336,7 +15339,7 @@
         <v>16</v>
       </c>
       <c r="C182" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D182" t="n">
         <v>2.275</v>
@@ -15356,7 +15359,7 @@
         <v>16</v>
       </c>
       <c r="C183" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D183" t="n">
         <v>2.969</v>
@@ -15376,7 +15379,7 @@
         <v>26</v>
       </c>
       <c r="C184" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D184" t="n">
         <v>2.205</v>
@@ -15396,7 +15399,7 @@
         <v>21</v>
       </c>
       <c r="C185" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D185" t="n">
         <v>1.3</v>
@@ -15416,7 +15419,7 @@
         <v>38</v>
       </c>
       <c r="C186" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D186" t="n">
         <v>3.4</v>
@@ -15436,7 +15439,7 @@
         <v>46</v>
       </c>
       <c r="C187" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D187" t="n">
         <v>2.767</v>
@@ -15456,7 +15459,7 @@
         <v>40</v>
       </c>
       <c r="C188" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D188" t="n">
         <v>3</v>
@@ -15476,7 +15479,7 @@
         <v>40</v>
       </c>
       <c r="C189" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D189" t="n">
         <v>2.536</v>
@@ -15496,7 +15499,7 @@
         <v>40</v>
       </c>
       <c r="C190" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D190" t="n">
         <v>3.721</v>
@@ -15516,7 +15519,7 @@
         <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D191" t="n">
         <v>3.727</v>
@@ -15536,7 +15539,7 @@
         <v>9</v>
       </c>
       <c r="C192" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D192" t="n">
         <v>2.686</v>
@@ -15556,7 +15559,7 @@
         <v>9</v>
       </c>
       <c r="C193" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D193" t="n">
         <v>3.844</v>
@@ -15576,7 +15579,7 @@
         <v>9</v>
       </c>
       <c r="C194" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D194" t="n">
         <v>2.967</v>
@@ -15596,7 +15599,7 @@
         <v>28</v>
       </c>
       <c r="C195" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D195" t="n">
         <v>3.647</v>
@@ -15616,7 +15619,7 @@
         <v>45</v>
       </c>
       <c r="C196" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D196" t="n">
         <v>3.354</v>
@@ -15636,7 +15639,7 @@
         <v>12</v>
       </c>
       <c r="C197" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D197" t="n">
         <v>2.737</v>
@@ -15656,7 +15659,7 @@
         <v>30</v>
       </c>
       <c r="C198" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D198" t="n">
         <v>1.611</v>
@@ -15676,7 +15679,7 @@
         <v>30</v>
       </c>
       <c r="C199" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D199" t="n">
         <v>2.911</v>
@@ -15696,7 +15699,7 @@
         <v>23</v>
       </c>
       <c r="C200" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D200" t="n">
         <v>2.868</v>
@@ -15716,7 +15719,7 @@
         <v>18</v>
       </c>
       <c r="C201" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D201" t="n">
         <v>2.344</v>
@@ -15736,7 +15739,7 @@
         <v>22</v>
       </c>
       <c r="C202" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D202" t="n">
         <v>3.167</v>
@@ -15756,7 +15759,7 @@
         <v>10</v>
       </c>
       <c r="C203" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D203" t="n">
         <v>3.514</v>
@@ -15776,7 +15779,7 @@
         <v>13</v>
       </c>
       <c r="C204" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D204" t="n">
         <v>3.133</v>
@@ -15796,7 +15799,7 @@
         <v>31</v>
       </c>
       <c r="C205" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D205" t="n">
         <v>2.406</v>
@@ -15816,7 +15819,7 @@
         <v>33</v>
       </c>
       <c r="C206" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D206" t="n">
         <v>2</v>
@@ -15836,7 +15839,7 @@
         <v>9</v>
       </c>
       <c r="C207" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D207" t="n">
         <v>2.406</v>
@@ -15856,7 +15859,7 @@
         <v>9</v>
       </c>
       <c r="C208" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D208" t="n">
         <v>2.918</v>
@@ -15876,7 +15879,7 @@
         <v>28</v>
       </c>
       <c r="C209" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D209" t="n">
         <v>3.251</v>
@@ -15896,7 +15899,7 @@
         <v>39</v>
       </c>
       <c r="C210" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D210" t="n">
         <v>3.091</v>
@@ -15916,7 +15919,7 @@
         <v>35</v>
       </c>
       <c r="C211" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D211" t="n">
         <v>3.182</v>
@@ -15936,7 +15939,7 @@
         <v>44</v>
       </c>
       <c r="C212" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D212" t="n">
         <v>2.786</v>
@@ -15956,7 +15959,7 @@
         <v>23</v>
       </c>
       <c r="C213" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D213" t="n">
         <v>2.825</v>
@@ -15976,7 +15979,7 @@
         <v>16</v>
       </c>
       <c r="C214" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D214" t="n">
         <v>3.388</v>
@@ -15996,7 +15999,7 @@
         <v>18</v>
       </c>
       <c r="C215" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D215" t="n">
         <v>2.14</v>
@@ -16016,7 +16019,7 @@
         <v>18</v>
       </c>
       <c r="C216" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D216" t="n">
         <v>3.464</v>
@@ -16036,7 +16039,7 @@
         <v>18</v>
       </c>
       <c r="C217" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D217" t="n">
         <v>3.14</v>
@@ -16056,7 +16059,7 @@
         <v>41</v>
       </c>
       <c r="C218" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D218" t="n">
         <v>2.563</v>
@@ -16076,7 +16079,7 @@
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D219" t="n">
         <v>3.7</v>
@@ -16096,7 +16099,7 @@
         <v>28</v>
       </c>
       <c r="C220" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D220" t="n">
         <v>3.182</v>
@@ -16116,7 +16119,7 @@
         <v>16</v>
       </c>
       <c r="C221" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D221" t="n">
         <v>2.34</v>
@@ -16136,7 +16139,7 @@
         <v>19</v>
       </c>
       <c r="C222" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D222" t="n">
         <v>2.841</v>
@@ -16156,7 +16159,7 @@
         <v>9</v>
       </c>
       <c r="C223" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D223" t="n">
         <v>3.6</v>
@@ -16176,7 +16179,7 @@
         <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D224" t="n">
         <v>3.5</v>
@@ -16196,13 +16199,13 @@
         <v>16</v>
       </c>
       <c r="C225" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D225" t="n">
         <v>2.889</v>
       </c>
       <c r="E225" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F225" t="n">
         <v>3.186</v>
@@ -16216,13 +16219,13 @@
         <v>16</v>
       </c>
       <c r="C226" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D226" t="n">
         <v>3.707</v>
       </c>
       <c r="E226" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F226" t="n">
         <v>3.644</v>
@@ -16236,13 +16239,13 @@
         <v>20</v>
       </c>
       <c r="C227" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D227" t="n">
         <v>2.885</v>
       </c>
       <c r="E227" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F227" t="n">
         <v>2.789</v>
@@ -16256,7 +16259,7 @@
         <v>23</v>
       </c>
       <c r="C228" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D228" t="n">
         <v>3.3</v>
@@ -16276,7 +16279,7 @@
         <v>46</v>
       </c>
       <c r="C229" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D229" t="n">
         <v>1.947</v>
@@ -16296,7 +16299,7 @@
         <v>24</v>
       </c>
       <c r="C230" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D230" t="n">
         <v>2.909</v>
@@ -16316,7 +16319,7 @@
         <v>38</v>
       </c>
       <c r="C231" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D231" t="n">
         <v>3.264</v>
@@ -16336,7 +16339,7 @@
         <v>34</v>
       </c>
       <c r="C232" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D232" t="n">
         <v>3.364</v>
@@ -16356,7 +16359,7 @@
         <v>29</v>
       </c>
       <c r="C233" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D233" t="n">
         <v>3.111</v>
@@ -16376,7 +16379,7 @@
         <v>16</v>
       </c>
       <c r="C234" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D234" t="n">
         <v>1.205</v>
@@ -16396,7 +16399,7 @@
         <v>20</v>
       </c>
       <c r="C235" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D235" t="n">
         <v>1.931</v>
@@ -16416,7 +16419,7 @@
         <v>21</v>
       </c>
       <c r="C236" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D236" t="n">
         <v>2.417</v>
@@ -16472,7 +16475,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" t="n">
         <v>1.945</v>
@@ -16492,7 +16495,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3" t="n">
         <v>3.258</v>
@@ -16512,7 +16515,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" t="n">
         <v>2.043</v>
@@ -16532,7 +16535,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="n">
         <v>3.587</v>
@@ -16552,7 +16555,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" t="n">
         <v>3.864</v>
@@ -16572,7 +16575,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" t="n">
         <v>2.481</v>
@@ -16592,7 +16595,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8" t="n">
         <v>3.4</v>
@@ -16612,7 +16615,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" t="n">
         <v>3.1</v>
@@ -16632,7 +16635,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="n">
         <v>2.136</v>
@@ -16652,7 +16655,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" t="n">
         <v>2.742</v>
@@ -16672,7 +16675,7 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12" t="n">
         <v>3.127</v>
@@ -16692,7 +16695,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D13" t="n">
         <v>4</v>
@@ -16712,7 +16715,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" t="n">
         <v>2.329</v>
@@ -16732,7 +16735,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" t="n">
         <v>3.261</v>
@@ -16752,7 +16755,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" t="n">
         <v>2.978</v>
@@ -16772,7 +16775,7 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" t="n">
         <v>1.978</v>
@@ -16792,7 +16795,7 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="n">
         <v>3.081</v>
@@ -16812,7 +16815,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" t="n">
         <v>3.305</v>
@@ -16832,7 +16835,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D20" t="n">
         <v>2.449</v>
@@ -16852,7 +16855,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D21" t="n">
         <v>2.217</v>
@@ -16872,7 +16875,7 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D22" t="n">
         <v>2.735</v>
@@ -16892,7 +16895,7 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D23" t="n">
         <v>2.424</v>
@@ -16912,7 +16915,7 @@
         <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" t="n">
         <v>3.531</v>
@@ -16932,7 +16935,7 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" t="n">
         <v>3.315</v>
@@ -16952,7 +16955,7 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" t="n">
         <v>2.702</v>
@@ -16972,7 +16975,7 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" t="n">
         <v>1.861</v>
@@ -16992,7 +16995,7 @@
         <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D28" t="n">
         <v>2.096</v>
@@ -17012,7 +17015,7 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D29" t="n">
         <v>3.161</v>
@@ -17032,7 +17035,7 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D30" t="n">
         <v>2.092</v>
@@ -17052,7 +17055,7 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" t="n">
         <v>2.236</v>
@@ -17072,7 +17075,7 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D32" t="n">
         <v>2.539</v>
@@ -17092,7 +17095,7 @@
         <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D33" t="n">
         <v>2.479</v>
@@ -17112,7 +17115,7 @@
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D34" t="n">
         <v>2.393</v>
@@ -17132,7 +17135,7 @@
         <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35" t="n">
         <v>1.9</v>
@@ -17152,7 +17155,7 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" t="n">
         <v>3.014</v>
@@ -17172,7 +17175,7 @@
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D37" t="n">
         <v>4</v>
@@ -17192,7 +17195,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D38" t="n">
         <v>3.903</v>
@@ -17212,7 +17215,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D39" t="n">
         <v>4</v>
@@ -17232,7 +17235,7 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D40" t="n">
         <v>2.959</v>
@@ -17252,7 +17255,7 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D41" t="n">
         <v>2.753</v>
@@ -17272,7 +17275,7 @@
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D42" t="n">
         <v>1.805</v>
@@ -17292,7 +17295,7 @@
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D43" t="n">
         <v>3.17</v>
@@ -17312,7 +17315,7 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D44" t="n">
         <v>2.724</v>
@@ -17332,7 +17335,7 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D45" t="n">
         <v>2.787</v>
@@ -17352,7 +17355,7 @@
         <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D46" t="n">
         <v>2.106</v>
@@ -17372,7 +17375,7 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D47" t="n">
         <v>3.18</v>
@@ -17392,7 +17395,7 @@
         <v>38</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D48" t="n">
         <v>3.211</v>
@@ -17412,7 +17415,7 @@
         <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D49" t="n">
         <v>2.803</v>
@@ -17432,7 +17435,7 @@
         <v>38</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D50" t="n">
         <v>2.667</v>
@@ -17452,7 +17455,7 @@
         <v>34</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D51" t="n">
         <v>3.4</v>
@@ -17472,7 +17475,7 @@
         <v>39</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D52" t="n">
         <v>2.628</v>
@@ -17492,7 +17495,7 @@
         <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D53" t="n">
         <v>2.067</v>
@@ -17512,7 +17515,7 @@
         <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D54" t="n">
         <v>2.962</v>
@@ -17532,7 +17535,7 @@
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D55" t="n">
         <v>3.458</v>
@@ -17552,7 +17555,7 @@
         <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D56" t="n">
         <v>3.55</v>
@@ -17572,7 +17575,7 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D57" t="n">
         <v>2.211</v>
@@ -17592,7 +17595,7 @@
         <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D58" t="n">
         <v>3.886</v>
@@ -17612,7 +17615,7 @@
         <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D59" t="n">
         <v>1.868</v>
@@ -17632,13 +17635,13 @@
         <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D60" t="n">
         <v>2.639</v>
       </c>
       <c r="E60" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F60" t="n">
         <v>2.42</v>
@@ -17652,13 +17655,13 @@
         <v>23</v>
       </c>
       <c r="C61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D61" t="n">
         <v>3.631</v>
       </c>
       <c r="E61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F61" t="n">
         <v>3.615</v>
@@ -17672,13 +17675,13 @@
         <v>18</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D62" t="n">
         <v>2.971</v>
       </c>
       <c r="E62" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F62" t="n">
         <v>3.073</v>
@@ -17692,7 +17695,7 @@
         <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D63" t="n">
         <v>2.254</v>
@@ -17712,7 +17715,7 @@
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D64" t="n">
         <v>2.597</v>
@@ -17732,7 +17735,7 @@
         <v>33</v>
       </c>
       <c r="C65" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D65" t="n">
         <v>3</v>
@@ -17752,7 +17755,7 @@
         <v>24</v>
       </c>
       <c r="C66" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D66" t="n">
         <v>2.35</v>
@@ -17772,7 +17775,7 @@
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D67" t="n">
         <v>2.7</v>
@@ -17792,7 +17795,7 @@
         <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D68" t="n">
         <v>3.859</v>
@@ -17812,7 +17815,7 @@
         <v>18</v>
       </c>
       <c r="C69" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D69" t="n">
         <v>3.048</v>
@@ -17832,7 +17835,7 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D70" t="n">
         <v>3.119</v>
@@ -17852,7 +17855,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D71" t="n">
         <v>2.244</v>
@@ -17872,7 +17875,7 @@
         <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D72" t="n">
         <v>2.83</v>
@@ -17892,7 +17895,7 @@
         <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D73" t="n">
         <v>2.951</v>
@@ -17912,7 +17915,7 @@
         <v>24</v>
       </c>
       <c r="C74" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D74" t="n">
         <v>3.07</v>
@@ -17932,7 +17935,7 @@
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D75" t="n">
         <v>3.934</v>
@@ -17952,7 +17955,7 @@
         <v>45</v>
       </c>
       <c r="C76" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D76" t="n">
         <v>3.079</v>
@@ -17972,7 +17975,7 @@
         <v>45</v>
       </c>
       <c r="C77" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D77" t="n">
         <v>2.676</v>
@@ -17992,7 +17995,7 @@
         <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D78" t="n">
         <v>2.959</v>
@@ -18012,7 +18015,7 @@
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D79" t="n">
         <v>2.213</v>
@@ -18032,7 +18035,7 @@
         <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D80" t="n">
         <v>2.214</v>
@@ -18052,7 +18055,7 @@
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D81" t="n">
         <v>2.939</v>
@@ -18072,7 +18075,7 @@
         <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D82" t="n">
         <v>2.325</v>
@@ -18092,7 +18095,7 @@
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D83" t="n">
         <v>3.19</v>
@@ -18112,7 +18115,7 @@
         <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D84" t="n">
         <v>2.5</v>
@@ -18132,7 +18135,7 @@
         <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D85" t="n">
         <v>2.72</v>
@@ -18152,7 +18155,7 @@
         <v>27</v>
       </c>
       <c r="C86" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D86" t="n">
         <v>2.444</v>
@@ -18172,7 +18175,7 @@
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D87" t="n">
         <v>3.417</v>
@@ -18192,7 +18195,7 @@
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D88" t="n">
         <v>2.861</v>
@@ -18212,7 +18215,7 @@
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D89" t="n">
         <v>2.239</v>
@@ -18232,7 +18235,7 @@
         <v>29</v>
       </c>
       <c r="C90" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D90" t="n">
         <v>2.855</v>
@@ -18252,7 +18255,7 @@
         <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D91" t="n">
         <v>2.263</v>
@@ -18272,7 +18275,7 @@
         <v>14</v>
       </c>
       <c r="C92" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D92" t="n">
         <v>3.164</v>
@@ -18292,7 +18295,7 @@
         <v>34</v>
       </c>
       <c r="C93" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D93" t="n">
         <v>3.39</v>
@@ -18312,7 +18315,7 @@
         <v>18</v>
       </c>
       <c r="C94" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D94" t="n">
         <v>3.548</v>
@@ -18332,7 +18335,7 @@
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D95" t="n">
         <v>3.061</v>
@@ -18352,7 +18355,7 @@
         <v>18</v>
       </c>
       <c r="C96" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D96" t="n">
         <v>3.452</v>
@@ -18372,7 +18375,7 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D97" t="n">
         <v>2.03</v>
@@ -18392,7 +18395,7 @@
         <v>33</v>
       </c>
       <c r="C98" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D98" t="n">
         <v>4</v>
@@ -18412,7 +18415,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D99" t="n">
         <v>2.156</v>
@@ -18432,7 +18435,7 @@
         <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D100" t="n">
         <v>2.826</v>
@@ -18452,7 +18455,7 @@
         <v>18</v>
       </c>
       <c r="C101" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D101" t="n">
         <v>2.79</v>
@@ -18472,7 +18475,7 @@
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D102" t="n">
         <v>2.8</v>
@@ -18492,7 +18495,7 @@
         <v>38</v>
       </c>
       <c r="C103" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D103" t="n">
         <v>2.368</v>
@@ -18512,13 +18515,13 @@
         <v>34</v>
       </c>
       <c r="C104" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D104" t="n">
         <v>2.468</v>
       </c>
       <c r="E104" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F104" t="n">
         <v>2.387</v>
@@ -18532,7 +18535,7 @@
         <v>24</v>
       </c>
       <c r="C105" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D105" t="n">
         <v>2.167</v>
@@ -18552,7 +18555,7 @@
         <v>44</v>
       </c>
       <c r="C106" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D106" t="n">
         <v>2.179</v>
@@ -18572,7 +18575,7 @@
         <v>38</v>
       </c>
       <c r="C107" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D107" t="n">
         <v>2.488</v>
@@ -18592,7 +18595,7 @@
         <v>16</v>
       </c>
       <c r="C108" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D108" t="n">
         <v>2.817</v>
@@ -18612,7 +18615,7 @@
         <v>20</v>
       </c>
       <c r="C109" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D109" t="n">
         <v>2.667</v>
@@ -18632,7 +18635,7 @@
         <v>20</v>
       </c>
       <c r="C110" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D110" t="n">
         <v>3.292</v>
@@ -18688,7 +18691,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="n">
         <v>3.971</v>
@@ -18708,7 +18711,7 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="n">
         <v>2.728</v>
@@ -18728,7 +18731,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" t="n">
         <v>2.689</v>
@@ -18748,7 +18751,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" t="n">
         <v>3.483</v>
@@ -18768,7 +18771,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
         <v>3.32</v>
@@ -18788,7 +18791,7 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="n">
         <v>3.244</v>
@@ -18808,7 +18811,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" t="n">
         <v>3.286</v>
@@ -18828,7 +18831,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" t="n">
         <v>3.294</v>
@@ -18848,7 +18851,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="n">
         <v>2.73</v>
@@ -18868,7 +18871,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" t="n">
         <v>2.397</v>
@@ -18888,7 +18891,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" t="n">
         <v>2.811</v>
@@ -18908,7 +18911,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D13" t="n">
         <v>2.916</v>
@@ -18928,7 +18931,7 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" t="n">
         <v>3.593</v>
@@ -18948,7 +18951,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" t="n">
         <v>2.471</v>
@@ -18968,7 +18971,7 @@
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" t="n">
         <v>2.323</v>
@@ -18988,7 +18991,7 @@
         <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" t="n">
         <v>2.955</v>
@@ -19008,7 +19011,7 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" t="n">
         <v>3.527</v>
@@ -19028,7 +19031,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" t="n">
         <v>2.077</v>
@@ -19048,7 +19051,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" t="n">
         <v>3.065</v>
@@ -19068,7 +19071,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D21" t="n">
         <v>2.438</v>
@@ -19088,7 +19091,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D22" t="n">
         <v>1.696</v>
@@ -19108,7 +19111,7 @@
         <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" t="n">
         <v>2.627</v>
@@ -19128,7 +19131,7 @@
         <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" t="n">
         <v>2.77</v>
@@ -19148,7 +19151,7 @@
         <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D25" t="n">
         <v>2.97</v>
@@ -19168,7 +19171,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" t="n">
         <v>3.319</v>
@@ -19188,7 +19191,7 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" t="n">
         <v>3.532</v>
@@ -19208,7 +19211,7 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28" t="n">
         <v>2.131</v>
@@ -19228,7 +19231,7 @@
         <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D29" t="n">
         <v>3.099</v>
@@ -19248,7 +19251,7 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D30" t="n">
         <v>3.976</v>
@@ -19268,7 +19271,7 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D31" t="n">
         <v>3.204</v>
@@ -19288,7 +19291,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D32" t="n">
         <v>2.203</v>
@@ -19308,7 +19311,7 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D33" t="n">
         <v>2.635</v>
@@ -19328,7 +19331,7 @@
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D34" t="n">
         <v>1.933</v>
@@ -19348,7 +19351,7 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D35" t="n">
         <v>2.969</v>
@@ -19368,7 +19371,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D36" t="n">
         <v>3.55</v>
@@ -19388,7 +19391,7 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D37" t="n">
         <v>2.184</v>
@@ -19408,7 +19411,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D38" t="n">
         <v>3.474</v>
@@ -19428,7 +19431,7 @@
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D39" t="n">
         <v>2.658</v>
@@ -19448,7 +19451,7 @@
         <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D40" t="n">
         <v>2.539</v>
@@ -19468,7 +19471,7 @@
         <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D41" t="n">
         <v>3.557</v>
@@ -19488,7 +19491,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D42" t="n">
         <v>2.225</v>
@@ -19508,13 +19511,13 @@
         <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D43" t="n">
         <v>3.505</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F43" t="n">
         <v>3.366</v>
@@ -19528,7 +19531,7 @@
         <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" t="n">
         <v>1.681</v>
@@ -19548,7 +19551,7 @@
         <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D45" t="n">
         <v>2.496</v>
@@ -19568,7 +19571,7 @@
         <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D46" t="n">
         <v>3.49</v>
@@ -19588,7 +19591,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D47" t="n">
         <v>3.262</v>
@@ -19608,7 +19611,7 @@
         <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D48" t="n">
         <v>2.865</v>
@@ -19628,7 +19631,7 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D49" t="n">
         <v>2.544</v>
@@ -19648,7 +19651,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D50" t="n">
         <v>2.495</v>
@@ -19668,7 +19671,7 @@
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D51" t="n">
         <v>2.557</v>
@@ -19688,7 +19691,7 @@
         <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D52" t="n">
         <v>2.771</v>
@@ -19708,7 +19711,7 @@
         <v>32</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D53" t="n">
         <v>3.333</v>
@@ -19728,7 +19731,7 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D54" t="n">
         <v>3.759</v>
@@ -19748,7 +19751,7 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D55" t="n">
         <v>3.087</v>
@@ -19768,7 +19771,7 @@
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D56" t="n">
         <v>2.375</v>
@@ -19788,7 +19791,7 @@
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D57" t="n">
         <v>2.147</v>
@@ -19808,7 +19811,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D58" t="n">
         <v>2.564</v>
@@ -19828,7 +19831,7 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D59" t="n">
         <v>3.242</v>
@@ -19848,7 +19851,7 @@
         <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D60" t="n">
         <v>2.712</v>
@@ -19868,7 +19871,7 @@
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D61" t="n">
         <v>2.178</v>
@@ -19888,7 +19891,7 @@
         <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D62" t="n">
         <v>2.758</v>
@@ -19908,7 +19911,7 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D63" t="n">
         <v>3.099</v>
@@ -19928,7 +19931,7 @@
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D64" t="n">
         <v>3.523</v>
@@ -19948,7 +19951,7 @@
         <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D65" t="n">
         <v>3.327</v>
@@ -19968,7 +19971,7 @@
         <v>28</v>
       </c>
       <c r="C66" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D66" t="n">
         <v>2.333</v>
@@ -19988,7 +19991,7 @@
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D67" t="n">
         <v>2.186</v>
@@ -20008,7 +20011,7 @@
         <v>47</v>
       </c>
       <c r="C68" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D68" t="n">
         <v>2.903</v>
@@ -20028,7 +20031,7 @@
         <v>31</v>
       </c>
       <c r="C69" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D69" t="n">
         <v>1.996</v>
@@ -20048,7 +20051,7 @@
         <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D70" t="n">
         <v>2.386</v>

</xml_diff>